<commit_message>
rshiny + debut dashboard
</commit_message>
<xml_diff>
--- a/TMJA_moyennes.xlsx
+++ b/TMJA_moyennes.xlsx
@@ -5,19 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulfaguet/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulfaguet/Desktop/Projet-IA-Rhone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DFC85F56-0A1F-E848-901E-6BA2039BAEAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8225A405-A847-FB4E-AD0D-BE58A5EB0BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{CBBFD8B7-9DA8-DA43-9371-C3C50CAA4D75}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16760" xr2:uid="{CBBFD8B7-9DA8-DA43-9371-C3C50CAA4D75}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -117,339 +114,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="TMJA_A7"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="145">
-          <cell r="N145" t="str">
-            <v>TMJA T1</v>
-          </cell>
-          <cell r="O145" t="str">
-            <v>TMJA T2</v>
-          </cell>
-          <cell r="P145" t="str">
-            <v>TMJA T3</v>
-          </cell>
-          <cell r="R145" t="str">
-            <v>RatioPL T1</v>
-          </cell>
-          <cell r="S145" t="str">
-            <v>RatioPL T2</v>
-          </cell>
-          <cell r="T145" t="str">
-            <v>RatioPL T3</v>
-          </cell>
-          <cell r="V145" t="str">
-            <v>Nb PL T1</v>
-          </cell>
-          <cell r="W145" t="str">
-            <v>Nb PL T2</v>
-          </cell>
-          <cell r="X145" t="str">
-            <v>Nb PL T3</v>
-          </cell>
-        </row>
-        <row r="146">
-          <cell r="N146">
-            <v>95548.305555555562</v>
-          </cell>
-          <cell r="O146">
-            <v>70222.2</v>
-          </cell>
-          <cell r="P146">
-            <v>56793.25</v>
-          </cell>
-          <cell r="R146">
-            <v>13.191666666666666</v>
-          </cell>
-          <cell r="S146">
-            <v>16.82</v>
-          </cell>
-          <cell r="T146">
-            <v>14.074999999999999</v>
-          </cell>
-          <cell r="V146">
-            <v>12604.413974537038</v>
-          </cell>
-          <cell r="W146">
-            <v>11811.374040000001</v>
-          </cell>
-          <cell r="X146">
-            <v>7993.6499374999994</v>
-          </cell>
-        </row>
-        <row r="147">
-          <cell r="N147">
-            <v>93113.625</v>
-          </cell>
-          <cell r="O147">
-            <v>68745.75</v>
-          </cell>
-          <cell r="P147">
-            <v>57061</v>
-          </cell>
-          <cell r="R147">
-            <v>11.975000000000001</v>
-          </cell>
-          <cell r="S147">
-            <v>17.25</v>
-          </cell>
-          <cell r="T147">
-            <v>14.149999999999999</v>
-          </cell>
-          <cell r="V147">
-            <v>11150.356593750001</v>
-          </cell>
-          <cell r="W147">
-            <v>11858.641874999999</v>
-          </cell>
-          <cell r="X147">
-            <v>8074.1314999999995</v>
-          </cell>
-        </row>
-        <row r="148">
-          <cell r="N148">
-            <v>85224.71428571429</v>
-          </cell>
-          <cell r="O148">
-            <v>68623.199999999997</v>
-          </cell>
-          <cell r="P148">
-            <v>56026.5</v>
-          </cell>
-          <cell r="R148">
-            <v>12.042857142857143</v>
-          </cell>
-          <cell r="S148">
-            <v>16.740000000000002</v>
-          </cell>
-          <cell r="T148">
-            <v>14.075000000000001</v>
-          </cell>
-          <cell r="V148">
-            <v>10263.490591836735</v>
-          </cell>
-          <cell r="W148">
-            <v>11487.52368</v>
-          </cell>
-          <cell r="X148">
-            <v>7885.7298750000009</v>
-          </cell>
-        </row>
-        <row r="149">
-          <cell r="N149">
-            <v>92394.375</v>
-          </cell>
-          <cell r="O149">
-            <v>69220</v>
-          </cell>
-          <cell r="P149">
-            <v>56658.25</v>
-          </cell>
-          <cell r="R149">
-            <v>11.675000000000001</v>
-          </cell>
-          <cell r="S149">
-            <v>16.68</v>
-          </cell>
-          <cell r="T149">
-            <v>13.9</v>
-          </cell>
-          <cell r="V149">
-            <v>10787.04328125</v>
-          </cell>
-          <cell r="W149">
-            <v>11545.896000000001</v>
-          </cell>
-          <cell r="X149">
-            <v>7875.4967500000012</v>
-          </cell>
-        </row>
-        <row r="150">
-          <cell r="N150">
-            <v>91359.666666666672</v>
-          </cell>
-          <cell r="O150">
-            <v>72948.25</v>
-          </cell>
-          <cell r="P150">
-            <v>57475</v>
-          </cell>
-          <cell r="R150">
-            <v>12.377777777777778</v>
-          </cell>
-          <cell r="S150">
-            <v>16.2</v>
-          </cell>
-          <cell r="T150">
-            <v>13.725000000000001</v>
-          </cell>
-          <cell r="V150">
-            <v>11308.296518518518</v>
-          </cell>
-          <cell r="W150">
-            <v>11817.6165</v>
-          </cell>
-          <cell r="X150">
-            <v>7888.4437500000004</v>
-          </cell>
-        </row>
-        <row r="151">
-          <cell r="N151">
-            <v>93999.5</v>
-          </cell>
-          <cell r="O151">
-            <v>71960.800000000003</v>
-          </cell>
-          <cell r="P151">
-            <v>58637.75</v>
-          </cell>
-          <cell r="R151">
-            <v>11.612500000000001</v>
-          </cell>
-          <cell r="S151">
-            <v>17.04</v>
-          </cell>
-          <cell r="T151">
-            <v>13.8</v>
-          </cell>
-          <cell r="V151">
-            <v>10915.6919375</v>
-          </cell>
-          <cell r="W151">
-            <v>12262.12032</v>
-          </cell>
-          <cell r="X151">
-            <v>8092.009500000001</v>
-          </cell>
-        </row>
-        <row r="152">
-          <cell r="N152">
-            <v>90228.875</v>
-          </cell>
-          <cell r="O152">
-            <v>76670.5</v>
-          </cell>
-          <cell r="P152">
-            <v>59159.6</v>
-          </cell>
-          <cell r="R152">
-            <v>13.985714285714286</v>
-          </cell>
-          <cell r="S152">
-            <v>16.5</v>
-          </cell>
-          <cell r="T152">
-            <v>13.74</v>
-          </cell>
-          <cell r="V152">
-            <v>12619.152660714284</v>
-          </cell>
-          <cell r="W152">
-            <v>12650.6325</v>
-          </cell>
-          <cell r="X152">
-            <v>8128.5290399999994</v>
-          </cell>
-        </row>
-        <row r="153">
-          <cell r="N153">
-            <v>86739.666666666672</v>
-          </cell>
-          <cell r="O153">
-            <v>77732.5</v>
-          </cell>
-          <cell r="P153">
-            <v>61456</v>
-          </cell>
-          <cell r="R153">
-            <v>15.5</v>
-          </cell>
-          <cell r="S153">
-            <v>16.95</v>
-          </cell>
-          <cell r="T153">
-            <v>14.125</v>
-          </cell>
-          <cell r="V153">
-            <v>13444.648333333334</v>
-          </cell>
-          <cell r="W153">
-            <v>13175.658749999999</v>
-          </cell>
-          <cell r="X153">
-            <v>8680.66</v>
-          </cell>
-        </row>
-        <row r="154">
-          <cell r="N154">
-            <v>89193.166666666672</v>
-          </cell>
-          <cell r="O154">
-            <v>74282.8</v>
-          </cell>
-          <cell r="P154">
-            <v>63210.5</v>
-          </cell>
-          <cell r="R154">
-            <v>15.453333333333333</v>
-          </cell>
-          <cell r="S154">
-            <v>18.017999999999997</v>
-          </cell>
-          <cell r="T154">
-            <v>15.094999999999999</v>
-          </cell>
-          <cell r="V154">
-            <v>13783.317355555555</v>
-          </cell>
-          <cell r="W154">
-            <v>13384.274904</v>
-          </cell>
-          <cell r="X154">
-            <v>9541.6249750000006</v>
-          </cell>
-        </row>
-        <row r="155">
-          <cell r="N155">
-            <v>97765.6</v>
-          </cell>
-          <cell r="O155">
-            <v>77280</v>
-          </cell>
-          <cell r="P155">
-            <v>64838.166666666664</v>
-          </cell>
-          <cell r="R155">
-            <v>13.738</v>
-          </cell>
-          <cell r="S155">
-            <v>17.618000000000002</v>
-          </cell>
-          <cell r="T155">
-            <v>15.061666666666666</v>
-          </cell>
-          <cell r="V155">
-            <v>13431.038128</v>
-          </cell>
-          <cell r="W155">
-            <v>13615.190400000003</v>
-          </cell>
-          <cell r="X155">
-            <v>9765.7085361111094</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -749,15 +413,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99563AD2-5FA4-6349-8F20-D249E49DE2DE}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -767,26 +431,26 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2010</v>
       </c>
@@ -799,26 +463,26 @@
       <c r="D2">
         <v>56793.25</v>
       </c>
+      <c r="E2">
+        <v>13.191666666666666</v>
+      </c>
       <c r="F2">
-        <v>13.191666666666666</v>
+        <v>16.82</v>
       </c>
       <c r="G2">
-        <v>16.82</v>
+        <v>14.074999999999999</v>
       </c>
       <c r="H2">
-        <v>14.074999999999999</v>
+        <v>12604.413974537038</v>
+      </c>
+      <c r="I2">
+        <v>11811.374040000001</v>
       </c>
       <c r="J2">
-        <v>12604.413974537038</v>
-      </c>
-      <c r="K2">
-        <v>11811.374040000001</v>
-      </c>
-      <c r="L2">
         <v>7993.6499374999994</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2011</v>
       </c>
@@ -831,26 +495,26 @@
       <c r="D3">
         <v>57061</v>
       </c>
+      <c r="E3">
+        <v>11.975000000000001</v>
+      </c>
       <c r="F3">
-        <v>11.975000000000001</v>
+        <v>17.25</v>
       </c>
       <c r="G3">
-        <v>17.25</v>
+        <v>14.149999999999999</v>
       </c>
       <c r="H3">
-        <v>14.149999999999999</v>
+        <v>11150.356593750001</v>
+      </c>
+      <c r="I3">
+        <v>11858.641874999999</v>
       </c>
       <c r="J3">
-        <v>11150.356593750001</v>
-      </c>
-      <c r="K3">
-        <v>11858.641874999999</v>
-      </c>
-      <c r="L3">
         <v>8074.1314999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2012</v>
       </c>
@@ -863,26 +527,26 @@
       <c r="D4">
         <v>56026.5</v>
       </c>
+      <c r="E4">
+        <v>12.042857142857143</v>
+      </c>
       <c r="F4">
-        <v>12.042857142857143</v>
+        <v>16.740000000000002</v>
       </c>
       <c r="G4">
-        <v>16.740000000000002</v>
+        <v>14.075000000000001</v>
       </c>
       <c r="H4">
-        <v>14.075000000000001</v>
+        <v>10263.490591836735</v>
+      </c>
+      <c r="I4">
+        <v>11487.52368</v>
       </c>
       <c r="J4">
-        <v>10263.490591836735</v>
-      </c>
-      <c r="K4">
-        <v>11487.52368</v>
-      </c>
-      <c r="L4">
         <v>7885.7298750000009</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2013</v>
       </c>
@@ -895,26 +559,26 @@
       <c r="D5">
         <v>56658.25</v>
       </c>
+      <c r="E5">
+        <v>11.675000000000001</v>
+      </c>
       <c r="F5">
-        <v>11.675000000000001</v>
+        <v>16.68</v>
       </c>
       <c r="G5">
-        <v>16.68</v>
+        <v>13.9</v>
       </c>
       <c r="H5">
-        <v>13.9</v>
+        <v>10787.04328125</v>
+      </c>
+      <c r="I5">
+        <v>11545.896000000001</v>
       </c>
       <c r="J5">
-        <v>10787.04328125</v>
-      </c>
-      <c r="K5">
-        <v>11545.896000000001</v>
-      </c>
-      <c r="L5">
         <v>7875.4967500000012</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2014</v>
       </c>
@@ -927,26 +591,26 @@
       <c r="D6">
         <v>57475</v>
       </c>
+      <c r="E6">
+        <v>12.377777777777778</v>
+      </c>
       <c r="F6">
-        <v>12.377777777777778</v>
+        <v>16.2</v>
       </c>
       <c r="G6">
-        <v>16.2</v>
+        <v>13.725000000000001</v>
       </c>
       <c r="H6">
-        <v>13.725000000000001</v>
+        <v>11308.296518518518</v>
+      </c>
+      <c r="I6">
+        <v>11817.6165</v>
       </c>
       <c r="J6">
-        <v>11308.296518518518</v>
-      </c>
-      <c r="K6">
-        <v>11817.6165</v>
-      </c>
-      <c r="L6">
         <v>7888.4437500000004</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2015</v>
       </c>
@@ -959,26 +623,26 @@
       <c r="D7">
         <v>58637.75</v>
       </c>
+      <c r="E7">
+        <v>11.612500000000001</v>
+      </c>
       <c r="F7">
-        <v>11.612500000000001</v>
+        <v>17.04</v>
       </c>
       <c r="G7">
-        <v>17.04</v>
+        <v>13.8</v>
       </c>
       <c r="H7">
-        <v>13.8</v>
+        <v>10915.6919375</v>
+      </c>
+      <c r="I7">
+        <v>12262.12032</v>
       </c>
       <c r="J7">
-        <v>10915.6919375</v>
-      </c>
-      <c r="K7">
-        <v>12262.12032</v>
-      </c>
-      <c r="L7">
         <v>8092.009500000001</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2016</v>
       </c>
@@ -991,26 +655,26 @@
       <c r="D8">
         <v>59159.6</v>
       </c>
+      <c r="E8">
+        <v>13.985714285714286</v>
+      </c>
       <c r="F8">
-        <v>13.985714285714286</v>
+        <v>16.5</v>
       </c>
       <c r="G8">
-        <v>16.5</v>
+        <v>13.74</v>
       </c>
       <c r="H8">
-        <v>13.74</v>
+        <v>12619.152660714284</v>
+      </c>
+      <c r="I8">
+        <v>12650.6325</v>
       </c>
       <c r="J8">
-        <v>12619.152660714284</v>
-      </c>
-      <c r="K8">
-        <v>12650.6325</v>
-      </c>
-      <c r="L8">
         <v>8128.5290399999994</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2017</v>
       </c>
@@ -1023,26 +687,26 @@
       <c r="D9">
         <v>61456</v>
       </c>
+      <c r="E9">
+        <v>15.5</v>
+      </c>
       <c r="F9">
-        <v>15.5</v>
+        <v>16.95</v>
       </c>
       <c r="G9">
-        <v>16.95</v>
+        <v>14.125</v>
       </c>
       <c r="H9">
-        <v>14.125</v>
+        <v>13444.648333333334</v>
+      </c>
+      <c r="I9">
+        <v>13175.658749999999</v>
       </c>
       <c r="J9">
-        <v>13444.648333333334</v>
-      </c>
-      <c r="K9">
-        <v>13175.658749999999</v>
-      </c>
-      <c r="L9">
         <v>8680.66</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2018</v>
       </c>
@@ -1055,26 +719,26 @@
       <c r="D10">
         <v>63210.5</v>
       </c>
+      <c r="E10">
+        <v>15.453333333333333</v>
+      </c>
       <c r="F10">
-        <v>15.453333333333333</v>
+        <v>18.017999999999997</v>
       </c>
       <c r="G10">
-        <v>18.017999999999997</v>
+        <v>15.094999999999999</v>
       </c>
       <c r="H10">
-        <v>15.094999999999999</v>
+        <v>13783.317355555555</v>
+      </c>
+      <c r="I10">
+        <v>13384.274904</v>
       </c>
       <c r="J10">
-        <v>13783.317355555555</v>
-      </c>
-      <c r="K10">
-        <v>13384.274904</v>
-      </c>
-      <c r="L10">
         <v>9541.6249750000006</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2019</v>
       </c>
@@ -1087,22 +751,22 @@
       <c r="D11">
         <v>64838.166666666664</v>
       </c>
+      <c r="E11">
+        <v>13.738</v>
+      </c>
       <c r="F11">
-        <v>13.738</v>
+        <v>17.618000000000002</v>
       </c>
       <c r="G11">
-        <v>17.618000000000002</v>
+        <v>15.061666666666666</v>
       </c>
       <c r="H11">
-        <v>15.061666666666666</v>
+        <v>13431.038128</v>
+      </c>
+      <c r="I11">
+        <v>13615.190400000003</v>
       </c>
       <c r="J11">
-        <v>13431.038128</v>
-      </c>
-      <c r="K11">
-        <v>13615.190400000003</v>
-      </c>
-      <c r="L11">
         <v>9765.7085361111094</v>
       </c>
     </row>

</xml_diff>